<commit_message>
dropdowns populated from flask
</commit_message>
<xml_diff>
--- a/Countries by region and centroid.xlsx
+++ b/Countries by region and centroid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjwal_000\Downloads\Programming\My Projects\Flight Sim Discovery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13EB050-AB51-452A-AEC5-AF4EF6E8725F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39328E42-B021-4BD4-8399-A6EFE8BF85F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29760" yWindow="510" windowWidth="15135" windowHeight="20160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7605" yWindow="3780" windowWidth="15135" windowHeight="17220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="countries" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="523">
   <si>
     <t>name</t>
   </si>
@@ -1588,6 +1588,18 @@
   </si>
   <si>
     <t>VietNam</t>
+  </si>
+  <si>
+    <t>Europe - Southern</t>
+  </si>
+  <si>
+    <t>Europe - Eastern</t>
+  </si>
+  <si>
+    <t>Africa - Eastern</t>
+  </si>
+  <si>
+    <t>Africa - Western</t>
   </si>
 </sst>
 </file>
@@ -1935,8 +1947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
-      <selection activeCell="A236" sqref="A236"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5560,7 +5572,7 @@
         <v>6</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>501</v>
+        <v>520</v>
       </c>
       <c r="E181" s="1">
         <v>45.943161000000003</v>
@@ -5580,7 +5592,7 @@
         <v>6</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>501</v>
+        <v>520</v>
       </c>
       <c r="E182" s="1">
         <v>61.524009999999997</v>
@@ -5600,7 +5612,7 @@
         <v>11</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>506</v>
+        <v>521</v>
       </c>
       <c r="E183" s="1">
         <v>-1.9402779999999999</v>
@@ -5640,7 +5652,7 @@
         <v>11</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>503</v>
+        <v>522</v>
       </c>
       <c r="E185" s="1">
         <v>-24.143474000000001</v>
@@ -6080,7 +6092,7 @@
         <v>6</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>496</v>
+        <v>519</v>
       </c>
       <c r="E207" s="1">
         <v>40.463667000000001</v>

</xml_diff>